<commit_message>
Habilitación de control de roles para los usuarios
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACIÓN/1.6 Backlog/G1_Backlog_V3.0.0.xlsx
+++ b/PREGAME/1. ELICITACIÓN/1.6 Backlog/G1_Backlog_V3.0.0.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\QUINTO SEMESTRE MAYO 23 - SEPTIEMBRE 23\NahirCarrera_14765_G1_MPSW\PREGAME\1. ELICITACIÓN\1.6 Backlog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\Uni\HostProyectos\PROCESOS\NahirCarrera_14765_G1_MPSW\PREGAME\1. ELICITACIÓN\1.6 Backlog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E20AB4BF-B529-4574-A77A-0BE4D70F17D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0AB6B24-85B8-4F8A-88BE-98E179B5D304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="674" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="674" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -21,6 +21,17 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -959,7 +970,7 @@
                 <a:latin typeface="Roboto"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="2087969067"/>
@@ -1035,7 +1046,7 @@
                 <a:latin typeface="Roboto"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="es-EC"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="416555524"/>
@@ -1058,7 +1069,7 @@
               <a:latin typeface="Roboto"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="es-EC"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2670,8 +2681,8 @@
   </sheetPr>
   <dimension ref="B1:I993"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5197,7 +5208,7 @@
   </sheetPr>
   <dimension ref="A1:Q1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="74" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView topLeftCell="A42" zoomScale="74" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="O61" sqref="O61"/>
     </sheetView>
   </sheetViews>

</xml_diff>